<commit_message>
feat(phase11): Compléter onglet 1 Transactions + Initialisation mappings autorisés + Logging backend
- Onglet 1 (Transactions) : Backend, Frontend et Migration complétés
- Initialisation automatique des mappings autorisés lors de la création d'une propriété
- Configuration logging backend pour capturer toutes les erreurs dans logs/backend_*.log
- Mise à jour MD pour refléter l'état réel (onglet 1 complété)
- Correction isolation mappings autorisés par propriété
- Ajout logs détaillés pour debugging (backend, API, frontend)
</commit_message>
<xml_diff>
--- a/backend/data/input/trades/mappings_2026-01-19.xlsx
+++ b/backend/data/input/trades/mappings_2026-01-19.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisgarnier/Desktop/LMNP/Evry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9023CB31-F260-1E48-A02D-9A7C076C9501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E445681-3E7A-EA48-8BC1-8B678F6F4C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="1880" windowWidth="26440" windowHeight="15440" xr2:uid="{4A625602-8C96-7D4B-BADC-8EADE9CB5A8C}"/>
   </bookViews>
   <sheets>
     <sheet name="mappings_2026-01-19" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'mappings_2026-01-19'!$A$1:$I$170</definedName>
+  </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1563,10 +1566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABC6AF2-832D-E247-A55E-AD378F29BB93}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1600,7 +1604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1629,7 +1633,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1658,7 +1662,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1745,7 +1749,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1803,7 +1807,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1890,7 +1894,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1919,7 +1923,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1948,7 +1952,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1977,7 +1981,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2006,7 +2010,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2064,7 +2068,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2093,7 +2097,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2151,7 +2155,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2180,7 +2184,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2209,7 +2213,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2238,7 +2242,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2267,7 +2271,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2296,7 +2300,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2325,7 +2329,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2354,7 +2358,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2383,7 +2387,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2412,7 +2416,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2470,7 +2474,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2528,7 +2532,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2557,7 +2561,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2586,7 +2590,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2615,7 +2619,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2644,7 +2648,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2673,7 +2677,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2702,7 +2706,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2731,7 +2735,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2760,7 +2764,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2847,7 +2851,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2876,7 +2880,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2905,7 +2909,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2934,7 +2938,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2963,7 +2967,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2992,7 +2996,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3021,7 +3025,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3050,7 +3054,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3079,7 +3083,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3108,7 +3112,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3137,7 +3141,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3166,7 +3170,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3195,7 +3199,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3224,7 +3228,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3253,7 +3257,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3282,7 +3286,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3311,7 +3315,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3340,7 +3344,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3369,7 +3373,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3398,7 +3402,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3427,7 +3431,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3456,7 +3460,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3514,7 +3518,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3543,7 +3547,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3572,7 +3576,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3601,7 +3605,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3630,7 +3634,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3659,7 +3663,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3688,7 +3692,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3717,7 +3721,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3746,7 +3750,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3775,7 +3779,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3804,7 +3808,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3833,7 +3837,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3862,7 +3866,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3891,7 +3895,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3949,7 +3953,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3978,7 +3982,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4007,7 +4011,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4036,7 +4040,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4065,7 +4069,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4094,7 +4098,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4123,7 +4127,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4152,7 +4156,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4181,7 +4185,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4210,7 +4214,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4239,7 +4243,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4268,7 +4272,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4297,7 +4301,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4326,7 +4330,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4355,7 +4359,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4384,7 +4388,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4413,7 +4417,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4442,7 +4446,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4471,7 +4475,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4500,7 +4504,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4529,7 +4533,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4558,7 +4562,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4587,7 +4591,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4616,7 +4620,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4645,7 +4649,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4674,7 +4678,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4703,7 +4707,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4732,7 +4736,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4761,7 +4765,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4790,7 +4794,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4819,7 +4823,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4848,7 +4852,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4877,7 +4881,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4906,7 +4910,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4935,7 +4939,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4964,7 +4968,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4993,7 +4997,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5022,7 +5026,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5051,7 +5055,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5080,7 +5084,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5109,7 +5113,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5138,7 +5142,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5167,7 +5171,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5196,7 +5200,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5225,7 +5229,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5254,7 +5258,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5283,7 +5287,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5312,7 +5316,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5341,7 +5345,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5370,7 +5374,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5399,7 +5403,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5428,7 +5432,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5457,7 +5461,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5486,7 +5490,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5515,7 +5519,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5544,7 +5548,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5573,7 +5577,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5602,7 +5606,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5631,7 +5635,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5660,7 +5664,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5689,7 +5693,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5718,7 +5722,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5747,7 +5751,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5776,7 +5780,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5805,7 +5809,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5834,7 +5838,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5892,7 +5896,7 @@
         <v>46041.602430555555</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5921,7 +5925,7 @@
         <v>46041.604189814818</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5950,7 +5954,7 @@
         <v>46041.604409722226</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5979,7 +5983,7 @@
         <v>46041.604467592595</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6008,7 +6012,7 @@
         <v>46041.604513888888</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -6037,7 +6041,7 @@
         <v>46041.604560185187</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6066,7 +6070,7 @@
         <v>46041.60460648148</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6095,7 +6099,7 @@
         <v>46041.60465277778</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6124,7 +6128,7 @@
         <v>46041.604722222219</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6153,7 +6157,7 @@
         <v>46041.604756944442</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6182,7 +6186,7 @@
         <v>46041.604803240742</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6211,7 +6215,7 @@
         <v>46041.604849537034</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6240,7 +6244,7 @@
         <v>46041.60491898148</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6269,7 +6273,7 @@
         <v>46041.60496527778</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6298,7 +6302,7 @@
         <v>46041.605011574073</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6327,7 +6331,7 @@
         <v>46041.605069444442</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6356,7 +6360,7 @@
         <v>46041.605138888888</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6385,7 +6389,7 @@
         <v>46041.605185185188</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6414,7 +6418,7 @@
         <v>46041.605254629627</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6443,7 +6447,7 @@
         <v>46041.605312500003</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6472,7 +6476,7 @@
         <v>46041.605405092596</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6502,6 +6506,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I170" xr:uid="{AABC6AF2-832D-E247-A55E-AD378F29BB93}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Emprunt"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{8a46d01b-cbcd-481a-a2d1-30a340e835f9}" enabled="1" method="Standard" siteId="{2fc24114-f31b-4c29-986a-6945244c7dc6}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>